<commit_message>
Finishes round one. Working code for pam, kmeans, hclust and mclust
</commit_message>
<xml_diff>
--- a/Solo1/reports/work.xlsx
+++ b/Solo1/reports/work.xlsx
@@ -5,14 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rahul/GDrive NU/450 Marketing/Solo1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rahul/GDrive NU/450 Marketing/github/Solo1/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="160" yWindow="7900" windowWidth="10360" windowHeight="8460" tabRatio="500"/>
+    <workbookView xWindow="40860" yWindow="-7560" windowWidth="23140" windowHeight="23560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Consolidations" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="95">
   <si>
     <t>q13</t>
   </si>
@@ -207,6 +208,111 @@
   </si>
   <si>
     <t>advisor</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>New Var</t>
+  </si>
+  <si>
+    <t>Old Vars</t>
+  </si>
+  <si>
+    <t>q13_visitfreq_social</t>
+  </si>
+  <si>
+    <t>q13_visitfreq_music</t>
+  </si>
+  <si>
+    <t>q13_visitfreq_video</t>
+  </si>
+  <si>
+    <t>r4, r7, r8, r9</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>r5, r6, r10, r12</t>
+  </si>
+  <si>
+    <t>r1, r2, r3, r11</t>
+  </si>
+  <si>
+    <t>q24_tech_posatt</t>
+  </si>
+  <si>
+    <t>q24_tech_negatv</t>
+  </si>
+  <si>
+    <t>r1,r2,r3,r5,r6</t>
+  </si>
+  <si>
+    <t>r7,r8</t>
+  </si>
+  <si>
+    <t>q24_tech_enter</t>
+  </si>
+  <si>
+    <t>q24_tech_comm</t>
+  </si>
+  <si>
+    <t>r10,r11,r12</t>
+  </si>
+  <si>
+    <t>r4,r9</t>
+  </si>
+  <si>
+    <t>q25_prsnlty_leader</t>
+  </si>
+  <si>
+    <t>q25_prsnlty_drive</t>
+  </si>
+  <si>
+    <t>r5,r7,r8</t>
+  </si>
+  <si>
+    <t>r1,r2,r3,r4</t>
+  </si>
+  <si>
+    <t>q25_prsnlty_risk</t>
+  </si>
+  <si>
+    <t>r9,r10,r11,r12</t>
+  </si>
+  <si>
+    <t>q25_prsnlty_follower</t>
+  </si>
+  <si>
+    <t>q26_shopsavvy_bargain</t>
+  </si>
+  <si>
+    <t>q26_shopsavvy_brands</t>
+  </si>
+  <si>
+    <t>q26_shopsavvy_earn2spend</t>
+  </si>
+  <si>
+    <t>q26_shopsavvy_applover</t>
+  </si>
+  <si>
+    <t>q26_shopsavvy_children</t>
+  </si>
+  <si>
+    <t>r3,r5</t>
+  </si>
+  <si>
+    <t>r7,r13,r14,r15,r18</t>
+  </si>
+  <si>
+    <t>r4,r13,r16</t>
+  </si>
+  <si>
+    <t>r6,r9,r8,r10,r12,r17</t>
   </si>
 </sst>
 </file>
@@ -533,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView zoomScale="179" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -985,4 +1091,225 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" t="s">
+        <v>93</v>
+      </c>
+      <c r="E16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Further work on report. Adds comparison between var sets.
</commit_message>
<xml_diff>
--- a/Solo1/reports/work.xlsx
+++ b/Solo1/reports/work.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="40860" yWindow="-7560" windowWidth="23140" windowHeight="23560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2460" yWindow="440" windowWidth="23140" windowHeight="15560" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Consolidations" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="111">
   <si>
     <t>q13</t>
   </si>
@@ -313,6 +314,54 @@
   </si>
   <si>
     <t>r6,r9,r8,r10,r12,r17</t>
+  </si>
+  <si>
+    <t>set1</t>
+  </si>
+  <si>
+    <t>set2</t>
+  </si>
+  <si>
+    <t>set3</t>
+  </si>
+  <si>
+    <t>hclust pc1-2 var</t>
+  </si>
+  <si>
+    <t>avg sil width</t>
+  </si>
+  <si>
+    <t>best k, sil width</t>
+  </si>
+  <si>
+    <t>ward.D</t>
+  </si>
+  <si>
+    <t>kmeans elbow</t>
+  </si>
+  <si>
+    <t>rsq</t>
+  </si>
+  <si>
+    <t>pam avg sil</t>
+  </si>
+  <si>
+    <t>best k</t>
+  </si>
+  <si>
+    <t>mclust k</t>
+  </si>
+  <si>
+    <t>lots of overlap</t>
+  </si>
+  <si>
+    <t>ward.D2</t>
+  </si>
+  <si>
+    <t>atleast one cluster has ~0 width</t>
+  </si>
+  <si>
+    <t>1 negative width</t>
   </si>
 </sst>
 </file>
@@ -1097,7 +1146,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -1312,4 +1361,206 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J1" t="s">
+        <v>100</v>
+      </c>
+      <c r="L1" t="s">
+        <v>104</v>
+      </c>
+      <c r="M1" t="s">
+        <v>105</v>
+      </c>
+      <c r="O1" t="s">
+        <v>106</v>
+      </c>
+      <c r="P1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2">
+        <v>28.3</v>
+      </c>
+      <c r="D2">
+        <v>9.3122079999999996E-2</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>6</v>
+      </c>
+      <c r="H2">
+        <v>0.27</v>
+      </c>
+      <c r="I2">
+        <v>0.11379431</v>
+      </c>
+      <c r="J2">
+        <v>6</v>
+      </c>
+      <c r="K2" t="s">
+        <v>109</v>
+      </c>
+      <c r="L2">
+        <v>0.10027680999999999</v>
+      </c>
+      <c r="M2">
+        <v>10</v>
+      </c>
+      <c r="N2" t="s">
+        <v>107</v>
+      </c>
+      <c r="O2">
+        <v>3</v>
+      </c>
+      <c r="P2">
+        <v>0.09</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3">
+        <v>31.87</v>
+      </c>
+      <c r="D3">
+        <v>0.12016014999999999</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
+      <c r="G3">
+        <v>8</v>
+      </c>
+      <c r="H3">
+        <v>0.13</v>
+      </c>
+      <c r="I3">
+        <v>0.13295109999999999</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>8.817055E-2</v>
+      </c>
+      <c r="M3">
+        <v>9</v>
+      </c>
+      <c r="N3" t="s">
+        <v>107</v>
+      </c>
+      <c r="O3">
+        <v>3</v>
+      </c>
+      <c r="P3">
+        <v>0.02</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4">
+        <v>25.22</v>
+      </c>
+      <c r="D4">
+        <v>0.06</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>6</v>
+      </c>
+      <c r="H4">
+        <v>0.28710000000000002</v>
+      </c>
+      <c r="I4">
+        <v>8.7773470000000006E-2</v>
+      </c>
+      <c r="J4">
+        <v>7</v>
+      </c>
+      <c r="L4">
+        <v>6.6646449999999996E-2</v>
+      </c>
+      <c r="M4">
+        <v>5</v>
+      </c>
+      <c r="O4">
+        <v>3</v>
+      </c>
+      <c r="P4">
+        <v>0.02</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Almost done with report
</commit_message>
<xml_diff>
--- a/Solo1/reports/work.xlsx
+++ b/Solo1/reports/work.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hw831\Documents\MSPA\450_marketing_analytics\Solo1\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rahul/GDrive NU/450 Marketing/github/Solo1/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="885" windowWidth="23145" windowHeight="15555" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="25600" yWindow="-7560" windowWidth="38400" windowHeight="23560" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,9 @@
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="142">
   <si>
     <t>q13</t>
   </si>
@@ -313,60 +316,12 @@
     <t>r6,r9,r8,r10,r12,r17</t>
   </si>
   <si>
-    <t>set1</t>
-  </si>
-  <si>
-    <t>set2</t>
-  </si>
-  <si>
-    <t>set3</t>
-  </si>
-  <si>
-    <t>hclust pc1-2 var</t>
-  </si>
-  <si>
-    <t>avg sil width</t>
-  </si>
-  <si>
-    <t>best k, sil width</t>
-  </si>
-  <si>
     <t>ward.D</t>
   </si>
   <si>
-    <t>kmeans elbow</t>
-  </si>
-  <si>
-    <t>rsq</t>
-  </si>
-  <si>
-    <t>pam avg sil</t>
-  </si>
-  <si>
-    <t>best k</t>
-  </si>
-  <si>
-    <t>mclust k</t>
-  </si>
-  <si>
-    <t>lots of overlap</t>
-  </si>
-  <si>
     <t>ward.D2</t>
   </si>
   <si>
-    <t>atleast one cluster has ~0 width</t>
-  </si>
-  <si>
-    <t>1 negative width</t>
-  </si>
-  <si>
-    <t>set4</t>
-  </si>
-  <si>
-    <t>good separation</t>
-  </si>
-  <si>
     <t>q1_age</t>
   </si>
   <si>
@@ -461,13 +416,55 @@
   </si>
   <si>
     <t>Aggregated Questions</t>
+  </si>
+  <si>
+    <t>Set ID</t>
+  </si>
+  <si>
+    <t>Linkage</t>
+  </si>
+  <si>
+    <t>VariationExplained_2PC</t>
+  </si>
+  <si>
+    <t>hclust_AvgSilWidth</t>
+  </si>
+  <si>
+    <t>AvgSilWidth_k</t>
+  </si>
+  <si>
+    <t>kmeans_Elbow</t>
+  </si>
+  <si>
+    <t>kmeans_Rsq</t>
+  </si>
+  <si>
+    <t>kmeans_AvgSilWidth</t>
+  </si>
+  <si>
+    <t>kmeans_k</t>
+  </si>
+  <si>
+    <t>pam_AvgSilWidth</t>
+  </si>
+  <si>
+    <t>pam_k</t>
+  </si>
+  <si>
+    <t>mclust_k</t>
+  </si>
+  <si>
+    <t>mclust_AvgSilWidth</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -480,6 +477,29 @@
       <u/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -502,14 +522,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -794,24 +821,24 @@
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.375" customWidth="1"/>
+    <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" customWidth="1"/>
     <col min="4" max="4" width="8.5" customWidth="1"/>
-    <col min="5" max="5" width="15.125" customWidth="1"/>
-    <col min="6" max="6" width="6.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.625" customWidth="1"/>
-    <col min="8" max="8" width="6.375" customWidth="1"/>
-    <col min="9" max="9" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="1.625" customWidth="1"/>
-    <col min="11" max="11" width="4.375" customWidth="1"/>
-    <col min="12" max="12" width="5.625" customWidth="1"/>
-    <col min="13" max="13" width="8.375" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" customWidth="1"/>
+    <col min="6" max="6" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" customWidth="1"/>
+    <col min="8" max="8" width="6.33203125" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="1.6640625" customWidth="1"/>
+    <col min="11" max="11" width="4.33203125" customWidth="1"/>
+    <col min="12" max="12" width="5.6640625" customWidth="1"/>
+    <col min="13" max="13" width="8.33203125" customWidth="1"/>
     <col min="14" max="14" width="1.5" customWidth="1"/>
-    <col min="15" max="15" width="4.375" customWidth="1"/>
-    <col min="16" max="16" width="5.625" customWidth="1"/>
+    <col min="15" max="15" width="4.33203125" customWidth="1"/>
+    <col min="16" max="16" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -1248,18 +1275,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.125" customWidth="1"/>
-    <col min="3" max="3" width="24.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.1640625" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="3.875" customWidth="1"/>
-    <col min="7" max="7" width="24.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.83203125" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
@@ -1276,19 +1303,19 @@
         <v>67</v>
       </c>
       <c r="G2" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="H2" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="I2" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="J2" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="K2" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
@@ -1305,7 +1332,7 @@
         <v>68</v>
       </c>
       <c r="G3" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="H3" t="s">
         <v>15</v>
@@ -1331,7 +1358,7 @@
         <v>68</v>
       </c>
       <c r="G4" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="J4" t="s">
         <v>15</v>
@@ -1348,7 +1375,7 @@
         <v>68</v>
       </c>
       <c r="G5" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="I5" t="s">
         <v>15</v>
@@ -1371,7 +1398,7 @@
         <v>68</v>
       </c>
       <c r="G6" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="H6" t="s">
         <v>15</v>
@@ -1394,7 +1421,7 @@
         <v>68</v>
       </c>
       <c r="G7" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="H7" t="s">
         <v>15</v>
@@ -1420,7 +1447,7 @@
         <v>68</v>
       </c>
       <c r="G8" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="H8" t="s">
         <v>15</v>
@@ -1446,7 +1473,7 @@
         <v>68</v>
       </c>
       <c r="G9" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="H9" t="s">
         <v>15</v>
@@ -1475,7 +1502,7 @@
         <v>68</v>
       </c>
       <c r="G10" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="J10" t="s">
         <v>15</v>
@@ -1779,7 +1806,7 @@
     </row>
     <row r="27" spans="3:11" x14ac:dyDescent="0.25">
       <c r="G27" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="H27" t="s">
         <v>15</v>
@@ -1790,7 +1817,7 @@
     </row>
     <row r="28" spans="3:11" x14ac:dyDescent="0.25">
       <c r="G28" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="H28" t="s">
         <v>15</v>
@@ -1801,7 +1828,7 @@
     </row>
     <row r="29" spans="3:11" x14ac:dyDescent="0.25">
       <c r="G29" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="H29" t="s">
         <v>15</v>
@@ -1812,7 +1839,7 @@
     </row>
     <row r="30" spans="3:11" x14ac:dyDescent="0.25">
       <c r="G30" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="J30" t="s">
         <v>15</v>
@@ -1820,7 +1847,7 @@
     </row>
     <row r="31" spans="3:11" x14ac:dyDescent="0.25">
       <c r="G31" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="J31" t="s">
         <v>15</v>
@@ -1828,7 +1855,7 @@
     </row>
     <row r="32" spans="3:11" x14ac:dyDescent="0.25">
       <c r="G32" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="J32" t="s">
         <v>15</v>
@@ -1836,7 +1863,7 @@
     </row>
     <row r="33" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G33" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="J33" t="s">
         <v>15</v>
@@ -1844,7 +1871,7 @@
     </row>
     <row r="34" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G34" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="J34" t="s">
         <v>15</v>
@@ -1852,7 +1879,7 @@
     </row>
     <row r="35" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G35" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="J35" t="s">
         <v>15</v>
@@ -1860,7 +1887,7 @@
     </row>
     <row r="36" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G36" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="J36" t="s">
         <v>15</v>
@@ -1868,23 +1895,23 @@
     </row>
     <row r="37" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G37" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="J37" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="7:10" x14ac:dyDescent="0.2">
       <c r="G38" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="J38" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="7:10" x14ac:dyDescent="0.2">
       <c r="G39" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="H39" t="s">
         <v>15</v>
@@ -1893,9 +1920,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="7:10" x14ac:dyDescent="0.2">
       <c r="G40" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="H40" t="s">
         <v>15</v>
@@ -1904,9 +1931,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="7:10" x14ac:dyDescent="0.2">
       <c r="G41" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="H41" t="s">
         <v>15</v>
@@ -1915,9 +1942,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="7:10" x14ac:dyDescent="0.2">
       <c r="G42" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="H42" t="s">
         <v>15</v>
@@ -1926,9 +1953,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="7:10" x14ac:dyDescent="0.2">
       <c r="G43" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="H43" t="s">
         <v>15</v>
@@ -1937,14 +1964,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="7:10" x14ac:dyDescent="0.2">
       <c r="G44" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="45" spans="7:10" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="45" spans="7:10" x14ac:dyDescent="0.2">
       <c r="G45" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="H45" t="s">
         <v>15</v>
@@ -1961,261 +1988,235 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" t="s">
+        <v>130</v>
+      </c>
       <c r="C1" t="s">
-        <v>98</v>
+        <v>131</v>
       </c>
       <c r="D1" t="s">
-        <v>99</v>
+        <v>132</v>
       </c>
       <c r="E1" t="s">
-        <v>100</v>
+        <v>133</v>
+      </c>
+      <c r="F1" t="s">
+        <v>134</v>
       </c>
       <c r="G1" t="s">
-        <v>102</v>
+        <v>135</v>
       </c>
       <c r="H1" t="s">
-        <v>103</v>
+        <v>136</v>
       </c>
       <c r="I1" t="s">
-        <v>99</v>
-      </c>
-      <c r="J1" t="s">
-        <v>100</v>
-      </c>
-      <c r="L1" t="s">
-        <v>104</v>
+        <v>137</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="K1" t="s">
+        <v>139</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>141</v>
       </c>
       <c r="M1" t="s">
-        <v>105</v>
-      </c>
-      <c r="O1" t="s">
-        <v>106</v>
-      </c>
-      <c r="P1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>95</v>
       </c>
-      <c r="B2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C2">
+      <c r="C2" s="4">
         <v>28.3</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <v>9.3122079999999996E-2</v>
       </c>
       <c r="E2">
         <v>5</v>
       </c>
-      <c r="G2">
+      <c r="F2">
         <v>6</v>
       </c>
-      <c r="H2">
+      <c r="G2" s="3">
         <v>0.27</v>
       </c>
+      <c r="H2" s="3">
+        <v>0.11379431</v>
+      </c>
       <c r="I2">
-        <v>0.11379431</v>
-      </c>
-      <c r="J2">
         <v>6</v>
       </c>
-      <c r="K2" t="s">
-        <v>109</v>
-      </c>
-      <c r="L2">
+      <c r="J2" s="3">
         <v>0.10027680999999999</v>
       </c>
+      <c r="K2">
+        <v>10</v>
+      </c>
+      <c r="L2" s="3">
+        <v>0.09</v>
+      </c>
       <c r="M2">
-        <v>10</v>
-      </c>
-      <c r="N2" t="s">
-        <v>107</v>
-      </c>
-      <c r="O2">
         <v>3</v>
       </c>
-      <c r="P2">
-        <v>0.09</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>96</v>
       </c>
-      <c r="B3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C3">
+      <c r="C3" s="4">
         <v>31.87</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>0.12016014999999999</v>
       </c>
       <c r="E3">
         <v>6</v>
       </c>
-      <c r="G3">
+      <c r="F3">
         <v>8</v>
       </c>
-      <c r="H3">
+      <c r="G3" s="3">
         <v>0.13</v>
       </c>
+      <c r="H3" s="3">
+        <v>0.13295109999999999</v>
+      </c>
       <c r="I3">
-        <v>0.13295109999999999</v>
-      </c>
-      <c r="J3">
         <v>2</v>
       </c>
-      <c r="L3">
+      <c r="J3" s="3">
         <v>8.817055E-2</v>
       </c>
+      <c r="K3">
+        <v>9</v>
+      </c>
+      <c r="L3" s="3">
+        <v>0.02</v>
+      </c>
       <c r="M3">
-        <v>9</v>
-      </c>
-      <c r="N3" t="s">
-        <v>107</v>
-      </c>
-      <c r="O3">
         <v>3</v>
       </c>
-      <c r="P3">
-        <v>0.02</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>97</v>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C4">
+        <v>96</v>
+      </c>
+      <c r="C4" s="4">
         <v>25.22</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>0.06</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
-      <c r="G4">
+      <c r="F4">
         <v>6</v>
       </c>
-      <c r="H4">
+      <c r="G4" s="3">
         <v>0.28710000000000002</v>
       </c>
+      <c r="H4" s="3">
+        <v>8.7773470000000006E-2</v>
+      </c>
       <c r="I4">
-        <v>8.7773470000000006E-2</v>
-      </c>
-      <c r="J4">
         <v>7</v>
       </c>
-      <c r="L4">
+      <c r="J4" s="3">
         <v>6.6646449999999996E-2</v>
       </c>
+      <c r="K4">
+        <v>5</v>
+      </c>
+      <c r="L4" s="3">
+        <v>0.02</v>
+      </c>
       <c r="M4">
-        <v>5</v>
-      </c>
-      <c r="O4">
         <v>3</v>
       </c>
-      <c r="P4">
-        <v>0.02</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>97</v>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C5">
-        <v>25.22</v>
-      </c>
-      <c r="D5">
-        <v>0.33500000000000002</v>
+        <v>95</v>
+      </c>
+      <c r="C5" s="4">
+        <v>40.200000000000003</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.14000000000000001</v>
       </c>
       <c r="E5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B6" t="s">
-        <v>101</v>
-      </c>
-      <c r="C6">
-        <v>40.200000000000003</v>
-      </c>
-      <c r="D6">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="E6">
+      <c r="F5">
+        <v>6</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0.15623337000000001</v>
+      </c>
+      <c r="I5">
         <v>2</v>
       </c>
-      <c r="G6">
-        <v>6</v>
-      </c>
-      <c r="H6">
-        <v>0.34599999999999997</v>
-      </c>
-      <c r="I6">
-        <v>0.15623337000000001</v>
-      </c>
-      <c r="J6">
+      <c r="J5" s="3">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="K5">
         <v>2</v>
       </c>
-      <c r="K6" t="s">
-        <v>112</v>
-      </c>
-      <c r="L6">
-        <v>0.13600000000000001</v>
-      </c>
-      <c r="M6">
-        <v>2</v>
+      <c r="L5" s="3">
+        <v>0.09</v>
+      </c>
+      <c r="M5">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>